<commit_message>
Implement first ex of SW06
</commit_message>
<xml_diff>
--- a/SW06/cnn-ex1-stud.xlsx
+++ b/SW06/cnn-ex1-stud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\src\jupyter\MSE-DeLearn\SW06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8B11AC-6F66-4416-8730-7D53A1693BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F8C57E-4B37-4289-87FC-8DB860348111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="2805" windowWidth="28800" windowHeight="15435" xr2:uid="{8C63438D-D797-2F4D-8C3D-BC6A238C5B67}"/>
+    <workbookView xWindow="20880" yWindow="3150" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{8C63438D-D797-2F4D-8C3D-BC6A238C5B67}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex 1-A" sheetId="2" r:id="rId1"/>
@@ -119,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +129,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,6 +212,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -524,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3AA706-F46E-BE45-8FC6-3A8A2D1CEA6E}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -695,35 +704,35 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <f>($C$6*C4+$D$6*D4+$E$6*E4)+C7</f>
+        <f>($C$6*C4+$D$6*D4+$E$6*E4)+$C$7</f>
         <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:J13" si="1">($C$6*D4+$D$6*E4+$E$6*F4)+D7</f>
-        <v>4</v>
+        <f>($C$6*D4+$D$6*E4+$E$6*F4)+$C$7</f>
+        <v>6</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>-6</v>
+        <f t="shared" ref="F13:K13" si="1">($C$6*E4+$D$6*F4+$E$6*G4)+$C$7</f>
+        <v>-4</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K13">
-        <f>($C$6*J4+$D$6*K4+$E$6*0)+$C$7</f>
+        <f>($C$6*J4+$D$6*K4)+$C$7</f>
         <v>6</v>
       </c>
     </row>
@@ -760,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D308E945-0386-A246-9572-FC8DE175F97D}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -774,7 +783,7 @@
     <col min="30" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
@@ -783,7 +792,7 @@
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K2" s="3" t="s">
         <v>6</v>
       </c>
@@ -795,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,9 +840,32 @@
       <c r="P3" s="2">
         <v>1</v>
       </c>
-      <c r="V3" s="5"/>
-    </row>
-    <row r="4" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="11">
+        <f>(D3*$K$3+E3*$L$3+D4*$K$4+E4*$L$4)+(D9*$K$6+E9*$L$6+D10*$K$7+E10*$L$7)+(D15*$K$9+E15*$L$9+D16*$K$10+E16*$L$10)+$L$12</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="11">
+        <f t="shared" ref="U3:V3" si="0">(E3*$K$3+F3*$L$3+E4*$K$4+F4*$L$4)+(E9*$K$6+F9*$L$6+E10*$K$7+F10*$L$7)+(E15*$K$9+F15*$L$9+E16*$K$10+F16*$L$10)+$L$12</f>
+        <v>1</v>
+      </c>
+      <c r="V3" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X3" s="11">
+        <f>(D3*$O$3+E3*$P$3+D4*$O$4+E4*$P$4)+(D9*$O$6+E9*$P$6+D10*$O$7+E10*$P$7)+(D15*$O$9+E15*$P$9+D16*$O$10+E16*$P$10)+$P$12</f>
+        <v>3</v>
+      </c>
+      <c r="Y3" s="11">
+        <f t="shared" ref="Y3:Z5" si="1">(E3*$O$3+F3*$P$3+E4*$O$4+F4*$P$4)+(E9*$O$6+F9*$P$6+E10*$O$7+F10*$P$7)+(E15*$O$9+F15*$P$9+E16*$O$10+F16*$P$10)+$P$12</f>
+        <v>2</v>
+      </c>
+      <c r="Z3" s="11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="2">
         <v>2</v>
       </c>
@@ -860,9 +892,32 @@
       <c r="P4" s="2">
         <v>0</v>
       </c>
-      <c r="V4" s="5"/>
-    </row>
-    <row r="5" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="11">
+        <f t="shared" ref="T4:T5" si="2">(D4*$K$3+E4*$L$3+D5*$K$4+E5*$L$4)+(D10*$K$6+E10*$L$6+D11*$K$7+E11*$L$7)+(D16*$K$9+E16*$L$9+D17*$K$10+E17*$L$10)+$L$12</f>
+        <v>3</v>
+      </c>
+      <c r="U4" s="11">
+        <f t="shared" ref="U4:U5" si="3">(E4*$K$3+F4*$L$3+E5*$K$4+F5*$L$4)+(E10*$K$6+F10*$L$6+E11*$K$7+F11*$L$7)+(E16*$K$9+F16*$L$9+E17*$K$10+F17*$L$10)+$L$12</f>
+        <v>-1</v>
+      </c>
+      <c r="V4" s="11">
+        <f t="shared" ref="V4:V5" si="4">(F4*$K$3+G4*$L$3+F5*$K$4+G5*$L$4)+(F10*$K$6+G10*$L$6+F11*$K$7+G11*$L$7)+(F16*$K$9+G16*$L$9+F17*$K$10+G17*$L$10)+$L$12</f>
+        <v>6</v>
+      </c>
+      <c r="X4" s="11">
+        <f t="shared" ref="X4:X5" si="5">(D4*$O$3+E4*$P$3+D5*$O$4+E5*$P$4)+(D10*$O$6+E10*$P$6+D11*$O$7+E11*$P$7)+(D16*$O$9+E16*$P$9+D17*$O$10+E17*$P$10)+$P$12</f>
+        <v>-1</v>
+      </c>
+      <c r="Y4" s="11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Z4" s="11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>0</v>
       </c>
@@ -879,9 +934,32 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="5"/>
-      <c r="V5" s="5"/>
-    </row>
-    <row r="6" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="11">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="U5" s="11">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="V5" s="11">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="Y5" s="11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Z5" s="11">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -912,7 +990,7 @@
       </c>
       <c r="V6" s="5"/>
     </row>
-    <row r="7" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -931,8 +1009,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -965,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <v>0</v>
       </c>
@@ -992,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <v>2</v>
       </c>
@@ -1007,7 +1085,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>1</v>
       </c>
@@ -1034,15 +1112,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1138,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <v>2</v>
       </c>

</xml_diff>